<commit_message>
testing word doc log1 commit
</commit_message>
<xml_diff>
--- a/My_Home_Meals.xlsx
+++ b/My_Home_Meals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\Google_Data_Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74724091-4D23-473A-BCAA-48FBB79B1AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2A6F22-CAC5-49BE-AA76-8A0F45972EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Home food?</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>yellow daal-aloo gobi-paneer pasanda-cahapti-rice-fish</t>
+  </si>
+  <si>
+    <t>idli-sambhar-chutney</t>
+  </si>
+  <si>
+    <t>After being a regular breakfast once/twice a week the speciality goes down.</t>
   </si>
 </sst>
 </file>
@@ -452,11 +458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,6 +566,26 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>44602.463287037041</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>